<commit_message>
إضافة حدث جديد في Card16 by admin at 2025-12-07 19:50:21
</commit_message>
<xml_diff>
--- a/l3.xlsx
+++ b/l3.xlsx
@@ -7612,61 +7612,17 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -7684,61 +7640,25 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
         <is>
           <t>21\7\2024</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -7756,61 +7676,17 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -7828,11 +7704,7 @@
           <t>550</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
           <t>✔</t>
@@ -7848,41 +7720,21 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
           <t>19\1\2025</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -7905,56 +7757,24 @@
           <t>573</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>8\4\2025</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -7977,36 +7797,16 @@
           <t>729</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8017,16 +7817,8 @@
           <t>7\7\2025</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -8054,36 +7846,12 @@
           <t>✅</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr">
         <is>
           <t>6/11/2025</t>
@@ -8121,11 +7889,7 @@
           <t>869</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
           <t>✔</t>
@@ -8136,41 +7900,17 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr">
         <is>
           <t>30\9\2025</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -8188,61 +7928,17 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -8260,61 +7956,17 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -8332,61 +7984,17 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N12" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -8404,61 +8012,17 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
-      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -13383,7 +12947,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13452,6 +13016,21 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Event</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Correction</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Servised by</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -13469,15 +13048,54 @@
           <t>150</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -13495,7 +13113,11 @@
           <t>300</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>✔</t>
@@ -13506,16 +13128,39 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
           <t>25\12\2024</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -13533,23 +13178,54 @@
           <t>450</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="J4" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L4" t="inlineStr">
         <is>
           <t>23\1\2025</t>
         </is>
       </c>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -13572,22 +13248,49 @@
           <t>497</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="H5" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L5" t="inlineStr">
         <is>
           <t>23\4\2025</t>
         </is>
       </c>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -13610,22 +13313,49 @@
           <t>696</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
           <t>✔</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L6" t="inlineStr">
         <is>
           <t>13\8\2025</t>
         </is>
       </c>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -13648,7 +13378,11 @@
           <t>808</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t xml:space="preserve"> ✔</t>
@@ -13659,15 +13393,34 @@
           <t>✔</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="L7" t="inlineStr">
         <is>
           <t>21\10\2025</t>
         </is>
       </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -13685,15 +13438,54 @@
           <t>1000</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -13711,15 +13503,54 @@
           <t>1150</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -13737,15 +13568,54 @@
           <t>1300</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -13763,15 +13633,54 @@
           <t>1450</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -13789,15 +13698,91 @@
           <t>1500</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>1\1\2024</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>سلك هالك</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>تم تغير سلك</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>م.رشدي</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>